<commit_message>
GOG-28 - Allow numeric values for external product code
</commit_message>
<xml_diff>
--- a/ReportService.Test/resources/pricelist_OK.xlsx
+++ b/ReportService.Test/resources/pricelist_OK.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlorusso\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dlorusso\github\gogas-excel-service\ReportService.Test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B617B709-029F-49B3-A83B-8272E18207D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2D1BA4-666B-4F42-A4F2-9F6D11E2461E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="222">
   <si>
     <t>Codice esterno</t>
   </si>
@@ -669,13 +669,7 @@
     <t>MAGESS102</t>
   </si>
   <si>
-    <t>MAGESS103</t>
-  </si>
-  <si>
     <t>Astuccio in legno + Magia di Primavera 10 ml in confezione regalo</t>
-  </si>
-  <si>
-    <t>MAGESS104</t>
   </si>
   <si>
     <t>9910</t>
@@ -781,7 +775,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -797,7 +791,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1120,10 +1114,10 @@
   <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C93" sqref="C93"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1191,8 +1185,8 @@
       <c r="B2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>215</v>
+      <c r="C2" s="6">
+        <v>9910</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>15</v>
@@ -1232,8 +1226,8 @@
       <c r="B3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>215</v>
+      <c r="C3" s="6">
+        <v>9910</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
@@ -1274,7 +1268,7 @@
         <v>45</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
@@ -1315,7 +1309,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -1356,7 +1350,7 @@
         <v>46</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
@@ -1397,7 +1391,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
@@ -1438,7 +1432,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
@@ -1479,7 +1473,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
@@ -1520,7 +1514,7 @@
         <v>49</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>15</v>
@@ -1561,7 +1555,7 @@
         <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
@@ -1602,7 +1596,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
@@ -1643,7 +1637,7 @@
         <v>61</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -1684,7 +1678,7 @@
         <v>65</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>15</v>
@@ -1725,7 +1719,7 @@
         <v>62</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>15</v>
@@ -1766,7 +1760,7 @@
         <v>51</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>15</v>
@@ -1807,7 +1801,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>15</v>
@@ -1848,7 +1842,7 @@
         <v>63</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>15</v>
@@ -1889,7 +1883,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>15</v>
@@ -1930,7 +1924,7 @@
         <v>64</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>15</v>
@@ -1971,7 +1965,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>15</v>
@@ -2012,7 +2006,7 @@
         <v>55</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>15</v>
@@ -2053,7 +2047,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>15</v>
@@ -2094,7 +2088,7 @@
         <v>83</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>15</v>
@@ -2135,7 +2129,7 @@
         <v>84</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>15</v>
@@ -2176,7 +2170,7 @@
         <v>85</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>15</v>
@@ -2217,7 +2211,7 @@
         <v>86</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>15</v>
@@ -2258,7 +2252,7 @@
         <v>87</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>15</v>
@@ -2299,7 +2293,7 @@
         <v>88</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
@@ -2340,7 +2334,7 @@
         <v>89</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>15</v>
@@ -2381,7 +2375,7 @@
         <v>90</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>15</v>
@@ -2422,7 +2416,7 @@
         <v>96</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>15</v>
@@ -2463,7 +2457,7 @@
         <v>91</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>15</v>
@@ -2504,7 +2498,7 @@
         <v>92</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>15</v>
@@ -2545,7 +2539,7 @@
         <v>93</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>15</v>
@@ -2586,7 +2580,7 @@
         <v>94</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>15</v>
@@ -2627,7 +2621,7 @@
         <v>95</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>15</v>
@@ -2668,7 +2662,7 @@
         <v>126</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>15</v>
@@ -2709,7 +2703,7 @@
         <v>127</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>15</v>
@@ -2750,7 +2744,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>15</v>
@@ -2791,7 +2785,7 @@
         <v>129</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>15</v>
@@ -2832,7 +2826,7 @@
         <v>130</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>15</v>
@@ -2873,7 +2867,7 @@
         <v>131</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>15</v>
@@ -2914,7 +2908,7 @@
         <v>132</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>15</v>
@@ -2955,7 +2949,7 @@
         <v>134</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>15</v>
@@ -2994,7 +2988,7 @@
         <v>135</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>15</v>
@@ -3033,7 +3027,7 @@
         <v>136</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>15</v>
@@ -3072,7 +3066,7 @@
         <v>137</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>15</v>
@@ -3111,7 +3105,7 @@
         <v>138</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>15</v>
@@ -3150,7 +3144,7 @@
         <v>141</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>15</v>
@@ -3189,7 +3183,7 @@
         <v>139</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>15</v>
@@ -3228,7 +3222,7 @@
         <v>140</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>15</v>
@@ -3267,7 +3261,7 @@
         <v>142</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>15</v>
@@ -3306,7 +3300,7 @@
         <v>143</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>15</v>
@@ -3345,7 +3339,7 @@
         <v>144</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>15</v>
@@ -3384,7 +3378,7 @@
         <v>145</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>15</v>
@@ -3423,7 +3417,7 @@
         <v>146</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>15</v>
@@ -3462,7 +3456,7 @@
         <v>147</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>15</v>
@@ -3501,7 +3495,7 @@
         <v>148</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>15</v>
@@ -3540,7 +3534,7 @@
         <v>151</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>15</v>
@@ -3579,7 +3573,7 @@
         <v>152</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>15</v>
@@ -3618,7 +3612,7 @@
         <v>153</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>15</v>
@@ -3657,7 +3651,7 @@
         <v>154</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>15</v>
@@ -3696,7 +3690,7 @@
         <v>155</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>15</v>
@@ -3735,7 +3729,7 @@
         <v>156</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>15</v>
@@ -3776,7 +3770,7 @@
         <v>163</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>15</v>
@@ -3817,7 +3811,7 @@
         <v>164</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>15</v>
@@ -3858,7 +3852,7 @@
         <v>165</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>15</v>
@@ -3899,7 +3893,7 @@
         <v>95</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>15</v>
@@ -3940,7 +3934,7 @@
         <v>170</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>15</v>
@@ -3981,7 +3975,7 @@
         <v>174</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>15</v>
@@ -4019,7 +4013,7 @@
         <v>175</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>15</v>
@@ -4057,7 +4051,7 @@
         <v>176</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>15</v>
@@ -4095,7 +4089,7 @@
         <v>177</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>15</v>
@@ -4133,7 +4127,7 @@
         <v>184</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>15</v>
@@ -4174,7 +4168,7 @@
         <v>185</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>15</v>
@@ -4215,7 +4209,7 @@
         <v>207</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>15</v>
@@ -4256,7 +4250,7 @@
         <v>186</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>15</v>
@@ -4297,7 +4291,7 @@
         <v>187</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>15</v>
@@ -4338,7 +4332,7 @@
         <v>188</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>15</v>
@@ -4379,7 +4373,7 @@
         <v>189</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>15</v>
@@ -4420,7 +4414,7 @@
         <v>190</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>15</v>
@@ -4458,7 +4452,7 @@
         <v>191</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>15</v>
@@ -4496,7 +4490,7 @@
         <v>192</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>15</v>
@@ -4534,7 +4528,7 @@
         <v>193</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>15</v>
@@ -4572,7 +4566,7 @@
         <v>194</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>15</v>
@@ -4610,7 +4604,7 @@
         <v>195</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>15</v>
@@ -4648,7 +4642,7 @@
         <v>196</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>15</v>
@@ -4686,7 +4680,7 @@
         <v>197</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>15</v>
@@ -4724,7 +4718,7 @@
         <v>210</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>15</v>
@@ -4758,14 +4752,14 @@
       </c>
     </row>
     <row r="91" spans="1:13" s="5" customFormat="1">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="2">
+        <v>103</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="C91" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>15</v>
@@ -4796,14 +4790,14 @@
       </c>
     </row>
     <row r="92" spans="1:13" s="5" customFormat="1">
-      <c r="A92" s="2" t="s">
-        <v>214</v>
+      <c r="A92" s="2">
+        <v>104</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>156</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>15</v>

</xml_diff>